<commit_message>
i18n of AttributeMetaData label
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="340" windowWidth="36220" windowHeight="17880" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37760" windowHeight="17880" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="org_molgenis_test_TypeTest" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="packages" sheetId="5" r:id="rId3"/>
     <sheet name="entities" sheetId="3" r:id="rId4"/>
     <sheet name="attributes" sheetId="4" r:id="rId5"/>
+    <sheet name="languages" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="188">
   <si>
     <t>text</t>
   </si>
@@ -551,6 +552,42 @@
   </si>
   <si>
     <t>xstringhidden</t>
+  </si>
+  <si>
+    <t>label.nl</t>
+  </si>
+  <si>
+    <t>waarde</t>
+  </si>
+  <si>
+    <t>label.en</t>
+  </si>
+  <si>
+    <t>label.de</t>
+  </si>
+  <si>
+    <t>Wert</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>nl</t>
+  </si>
+  <si>
+    <t>Nederlands</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>Deutsch</t>
   </si>
 </sst>
 </file>
@@ -606,9 +643,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -630,7 +668,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="16">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -644,6 +682,7 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -946,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR39"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="U1" workbookViewId="0">
       <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
@@ -5439,7 +5478,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD50"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5624,10 +5663,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S55"/>
+  <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5643,7 +5682,7 @@
     <col min="18" max="18" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5701,8 +5740,20 @@
       <c r="S1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="2" spans="1:19">
+      <c r="T1" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1" t="s">
+        <v>176</v>
+      </c>
+      <c r="V1" t="s">
+        <v>178</v>
+      </c>
+      <c r="W1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5721,8 +5772,20 @@
       <c r="K2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:19">
+      <c r="T2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>177</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -5745,7 +5808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -5765,7 +5828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -5788,7 +5851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -5811,7 +5874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
         <v>149</v>
       </c>
@@ -5828,7 +5891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
         <v>151</v>
       </c>
@@ -5854,7 +5917,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
         <v>152</v>
       </c>
@@ -5880,7 +5943,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:23">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -5903,7 +5966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:23">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -5926,7 +5989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:23">
       <c r="A12" t="s">
         <v>156</v>
       </c>
@@ -5952,7 +6015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:23">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -5975,7 +6038,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:23">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -5998,7 +6061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:23">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -6018,7 +6081,7 @@
         <v>42095</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:23">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -6923,4 +6986,57 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix #4600 Cannot import emx_all_datatypes.xlsx
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="340" windowWidth="36220" windowHeight="17880" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33580" windowHeight="16820" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="org_molgenis_test_TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="178">
   <si>
     <t>text</t>
   </si>
@@ -551,6 +551,12 @@
   </si>
   <si>
     <t>xstringhidden</t>
+  </si>
+  <si>
+    <t>2014-08-01</t>
+  </si>
+  <si>
+    <t>2015-04-01</t>
   </si>
 </sst>
 </file>
@@ -606,7 +612,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -622,15 +628,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -644,6 +651,8 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -946,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR39"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5613,7 +5622,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5626,8 +5634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="C12" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5991,8 +5999,8 @@
       <c r="F14" t="b">
         <v>0</v>
       </c>
-      <c r="H14" s="4">
-        <v>41852</v>
+      <c r="H14" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="N14" t="b">
         <v>1</v>
@@ -6014,8 +6022,8 @@
       <c r="F15" t="b">
         <v>1</v>
       </c>
-      <c r="H15" s="4">
-        <v>42095</v>
+      <c r="H15" s="1" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:19">

</xml_diff>

<commit_message>
Added labels and descriptions to all attributes
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="340" windowWidth="36220" windowHeight="17880" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33580" windowHeight="16060" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="org_molgenis_test_TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="283">
   <si>
     <t>text</t>
   </si>
@@ -551,6 +551,327 @@
   </si>
   <si>
     <t>xstringhidden</t>
+  </si>
+  <si>
+    <t>TypeTest identifer attribute</t>
+  </si>
+  <si>
+    <t>TypeTest boolean attribute</t>
+  </si>
+  <si>
+    <t>TypeTest nillable boolean attribute</t>
+  </si>
+  <si>
+    <t>TypeTest compound attribute</t>
+  </si>
+  <si>
+    <t>TypeTest compound int attribute</t>
+  </si>
+  <si>
+    <t>TypeTestRef value attribute</t>
+  </si>
+  <si>
+    <t>TypeTestRef label attribute</t>
+  </si>
+  <si>
+    <t>TypeTest compound string attribute</t>
+  </si>
+  <si>
+    <t>TypeTest categorical attribute</t>
+  </si>
+  <si>
+    <t>TypeTest nillable categorical attribute</t>
+  </si>
+  <si>
+    <t>TypeTest categorical mref attribute</t>
+  </si>
+  <si>
+    <t>TypeTest nillable categorical mref attribute</t>
+  </si>
+  <si>
+    <t>Typetest date attribute</t>
+  </si>
+  <si>
+    <t>Typetest nillable date attribute</t>
+  </si>
+  <si>
+    <t>Typetest datetime attribute</t>
+  </si>
+  <si>
+    <t>Typetest nillable datetime attribute</t>
+  </si>
+  <si>
+    <t>Typetest decimal attribute</t>
+  </si>
+  <si>
+    <t>Typetest nillable decimal attribute</t>
+  </si>
+  <si>
+    <t>Typetest email attribute</t>
+  </si>
+  <si>
+    <t>Typetest nillable email attribute</t>
+  </si>
+  <si>
+    <t>Typetest enum attribute</t>
+  </si>
+  <si>
+    <t>Typetest nillable enum attribute</t>
+  </si>
+  <si>
+    <t>Typetest html attribute</t>
+  </si>
+  <si>
+    <t>Typetest nillable html attribute</t>
+  </si>
+  <si>
+    <t>Typetest hyperlink attribute</t>
+  </si>
+  <si>
+    <t>Typetest nillable hyperlink attribute</t>
+  </si>
+  <si>
+    <t>Typetest int attribute</t>
+  </si>
+  <si>
+    <t>Typetest nillable int attribute</t>
+  </si>
+  <si>
+    <t>Typetest int range attribute</t>
+  </si>
+  <si>
+    <t>Typetest nillable intrange attribute</t>
+  </si>
+  <si>
+    <t>Typetest long attribute</t>
+  </si>
+  <si>
+    <t>Typetest nillable long attribute</t>
+  </si>
+  <si>
+    <t>Typetest longrange attribute</t>
+  </si>
+  <si>
+    <t>Typetest nillable longrange attribute</t>
+  </si>
+  <si>
+    <t>Typetest mref attribute</t>
+  </si>
+  <si>
+    <t>Typetest nillable mref attribute_value</t>
+  </si>
+  <si>
+    <t>Typetest string attribute</t>
+  </si>
+  <si>
+    <t>Typetest nillable string attribute</t>
+  </si>
+  <si>
+    <t>Typetest text attribute</t>
+  </si>
+  <si>
+    <t>Typetest nillable text attribute</t>
+  </si>
+  <si>
+    <t>Typetest xref attribute</t>
+  </si>
+  <si>
+    <t>Typetest nillable xref attribute_value</t>
+  </si>
+  <si>
+    <t>Typetest hidden string attribute</t>
+  </si>
+  <si>
+    <t>Typetest nillable hidden string attribute</t>
+  </si>
+  <si>
+    <t>Typetest unique string attribute</t>
+  </si>
+  <si>
+    <t>Typetest unique int attribute</t>
+  </si>
+  <si>
+    <t>Typetest unique xref attribute</t>
+  </si>
+  <si>
+    <t>Typetest computed xref attribute</t>
+  </si>
+  <si>
+    <t>Typetest computed int attribute</t>
+  </si>
+  <si>
+    <t>Location Chromosome attribute</t>
+  </si>
+  <si>
+    <t>Location Position attribute</t>
+  </si>
+  <si>
+    <t>Persion id attribute</t>
+  </si>
+  <si>
+    <t>Person age attribute</t>
+  </si>
+  <si>
+    <t>Person drivers licence attribute</t>
+  </si>
+  <si>
+    <t>value label</t>
+  </si>
+  <si>
+    <t>label label</t>
+  </si>
+  <si>
+    <t>id label</t>
+  </si>
+  <si>
+    <t>xbool label</t>
+  </si>
+  <si>
+    <t>xboolnillable label</t>
+  </si>
+  <si>
+    <t>xcompound label</t>
+  </si>
+  <si>
+    <t>xcompound_int label</t>
+  </si>
+  <si>
+    <t>xcompound_string label</t>
+  </si>
+  <si>
+    <t>xcategorical_value label</t>
+  </si>
+  <si>
+    <t>xcategoricalnillable_value label</t>
+  </si>
+  <si>
+    <t>xcategoricalmref_value label</t>
+  </si>
+  <si>
+    <t>xcatmrefnillable_value label</t>
+  </si>
+  <si>
+    <t>xdate label</t>
+  </si>
+  <si>
+    <t>xdatenillable label</t>
+  </si>
+  <si>
+    <t>xdatetime label</t>
+  </si>
+  <si>
+    <t>xdatetimenillable label</t>
+  </si>
+  <si>
+    <t>xdecimal label</t>
+  </si>
+  <si>
+    <t>xdecimalnillable label</t>
+  </si>
+  <si>
+    <t>xemail label</t>
+  </si>
+  <si>
+    <t>xemailnillable label</t>
+  </si>
+  <si>
+    <t>xenum label</t>
+  </si>
+  <si>
+    <t>xenumnillable label</t>
+  </si>
+  <si>
+    <t>xhtml label</t>
+  </si>
+  <si>
+    <t>xhtmlnillable label</t>
+  </si>
+  <si>
+    <t>xhyperlink label</t>
+  </si>
+  <si>
+    <t>xhyperlinknillable label</t>
+  </si>
+  <si>
+    <t>xint label</t>
+  </si>
+  <si>
+    <t>xintnillable label</t>
+  </si>
+  <si>
+    <t>xintrange label</t>
+  </si>
+  <si>
+    <t>xintrangenillable label</t>
+  </si>
+  <si>
+    <t>xlong label</t>
+  </si>
+  <si>
+    <t>xlongnillable label</t>
+  </si>
+  <si>
+    <t>xlongrange label</t>
+  </si>
+  <si>
+    <t>xlongrangenillable label</t>
+  </si>
+  <si>
+    <t>xmref_value label</t>
+  </si>
+  <si>
+    <t>xmrefnillable_value label</t>
+  </si>
+  <si>
+    <t>xstring label</t>
+  </si>
+  <si>
+    <t>xstringnillable label</t>
+  </si>
+  <si>
+    <t>xtext label</t>
+  </si>
+  <si>
+    <t>xtextnillable label</t>
+  </si>
+  <si>
+    <t>xxref_value label</t>
+  </si>
+  <si>
+    <t>xxrefnillable_value label</t>
+  </si>
+  <si>
+    <t>xstring_hidden label</t>
+  </si>
+  <si>
+    <t>xstringnillable_hidden label</t>
+  </si>
+  <si>
+    <t>xstring_unique label</t>
+  </si>
+  <si>
+    <t>xint_unique label</t>
+  </si>
+  <si>
+    <t>xxref_unique label</t>
+  </si>
+  <si>
+    <t>xcomputedxref label</t>
+  </si>
+  <si>
+    <t>xcomputedint label</t>
+  </si>
+  <si>
+    <t>Chromosome label</t>
+  </si>
+  <si>
+    <t>Position label</t>
+  </si>
+  <si>
+    <t>age label</t>
+  </si>
+  <si>
+    <t>driverslicence label</t>
   </si>
 </sst>
 </file>
@@ -606,9 +927,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -630,7 +953,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -644,6 +967,8 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -5425,7 +5750,6 @@
     <hyperlink ref="W38" r:id="rId124"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5613,7 +5937,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5624,10 +5947,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S55"/>
+  <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:U55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5640,10 +5963,11 @@
     <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.5" customWidth="1"/>
+    <col min="20" max="20" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5701,8 +6025,14 @@
       <c r="S1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="2" spans="1:19">
+      <c r="T1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5721,8 +6051,14 @@
       <c r="K2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:19">
+      <c r="T2" t="s">
+        <v>181</v>
+      </c>
+      <c r="U2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -5744,8 +6080,14 @@
       <c r="L3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="T3" t="s">
+        <v>182</v>
+      </c>
+      <c r="U3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -5764,8 +6106,14 @@
       <c r="M4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="T4" t="s">
+        <v>176</v>
+      </c>
+      <c r="U4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -5787,8 +6135,14 @@
       <c r="N5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="T5" t="s">
+        <v>177</v>
+      </c>
+      <c r="U5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -5810,8 +6164,14 @@
       <c r="N6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:19">
+      <c r="T6" t="s">
+        <v>178</v>
+      </c>
+      <c r="U6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>149</v>
       </c>
@@ -5827,8 +6187,14 @@
       <c r="F7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="T7" t="s">
+        <v>179</v>
+      </c>
+      <c r="U7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>151</v>
       </c>
@@ -5853,8 +6219,14 @@
       <c r="Q8" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="T8" t="s">
+        <v>180</v>
+      </c>
+      <c r="U8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>152</v>
       </c>
@@ -5879,8 +6251,14 @@
       <c r="Q9" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="10" spans="1:19">
+      <c r="T9" t="s">
+        <v>183</v>
+      </c>
+      <c r="U9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -5902,8 +6280,14 @@
       <c r="H10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:19">
+      <c r="T10" t="s">
+        <v>184</v>
+      </c>
+      <c r="U10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -5925,8 +6309,14 @@
       <c r="H11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:19">
+      <c r="T11" t="s">
+        <v>185</v>
+      </c>
+      <c r="U11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
         <v>156</v>
       </c>
@@ -5951,8 +6341,14 @@
       <c r="N12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:19">
+      <c r="T12" t="s">
+        <v>186</v>
+      </c>
+      <c r="U12" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -5974,8 +6370,14 @@
       <c r="H13" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="14" spans="1:19">
+      <c r="T13" t="s">
+        <v>187</v>
+      </c>
+      <c r="U13" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -5997,8 +6399,14 @@
       <c r="N14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:19">
+      <c r="T14" t="s">
+        <v>188</v>
+      </c>
+      <c r="U14" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -6017,8 +6425,14 @@
       <c r="H15" s="4">
         <v>42095</v>
       </c>
-    </row>
-    <row r="16" spans="1:19">
+      <c r="T15" t="s">
+        <v>189</v>
+      </c>
+      <c r="U15" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -6037,8 +6451,14 @@
       <c r="H16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="T16" t="s">
+        <v>190</v>
+      </c>
+      <c r="U16" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -6060,8 +6480,14 @@
       <c r="N17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="T17" t="s">
+        <v>191</v>
+      </c>
+      <c r="U17" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -6083,8 +6509,14 @@
       <c r="N18" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="T18" t="s">
+        <v>192</v>
+      </c>
+      <c r="U18" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -6103,8 +6535,14 @@
       <c r="H19">
         <v>15.666</v>
       </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="T19" t="s">
+        <v>193</v>
+      </c>
+      <c r="U19" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -6126,8 +6564,14 @@
       <c r="N20" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="T20" t="s">
+        <v>194</v>
+      </c>
+      <c r="U20" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -6146,8 +6590,14 @@
       <c r="H21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="T21" t="s">
+        <v>195</v>
+      </c>
+      <c r="U21" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -6172,8 +6622,14 @@
       <c r="N22" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:14">
+      <c r="T22" t="s">
+        <v>196</v>
+      </c>
+      <c r="U22" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -6195,8 +6651,14 @@
       <c r="H23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:14">
+      <c r="T23" t="s">
+        <v>197</v>
+      </c>
+      <c r="U23" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -6215,8 +6677,14 @@
       <c r="H24" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:14">
+      <c r="T24" t="s">
+        <v>198</v>
+      </c>
+      <c r="U24" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -6238,8 +6706,14 @@
       <c r="N25" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="T25" t="s">
+        <v>199</v>
+      </c>
+      <c r="U25" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -6261,8 +6735,14 @@
       <c r="N26" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="T26" t="s">
+        <v>200</v>
+      </c>
+      <c r="U26" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -6281,8 +6761,14 @@
       <c r="H27" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="T27" t="s">
+        <v>201</v>
+      </c>
+      <c r="U27" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -6304,8 +6790,14 @@
       <c r="N28" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="T28" t="s">
+        <v>202</v>
+      </c>
+      <c r="U28" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -6324,8 +6816,14 @@
       <c r="H29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="T29" t="s">
+        <v>203</v>
+      </c>
+      <c r="U29" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -6347,8 +6845,14 @@
       <c r="J30">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:14">
+      <c r="T30" t="s">
+        <v>204</v>
+      </c>
+      <c r="U30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -6370,8 +6874,14 @@
       <c r="I31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="T31" t="s">
+        <v>205</v>
+      </c>
+      <c r="U31" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -6390,8 +6900,14 @@
       <c r="H32">
         <v>12342151234</v>
       </c>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="T32" t="s">
+        <v>206</v>
+      </c>
+      <c r="U32" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -6410,8 +6926,14 @@
       <c r="H33">
         <v>12342151234</v>
       </c>
-    </row>
-    <row r="34" spans="1:16">
+      <c r="T33" t="s">
+        <v>207</v>
+      </c>
+      <c r="U33" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -6439,8 +6961,14 @@
       <c r="N34" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:16">
+      <c r="T34" t="s">
+        <v>208</v>
+      </c>
+      <c r="U34" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -6468,8 +6996,14 @@
       <c r="N35" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:16">
+      <c r="T35" t="s">
+        <v>209</v>
+      </c>
+      <c r="U35" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -6491,8 +7025,14 @@
       <c r="N36" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:16">
+      <c r="T36" t="s">
+        <v>210</v>
+      </c>
+      <c r="U36" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -6511,8 +7051,14 @@
       <c r="F37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:16">
+      <c r="T37" t="s">
+        <v>211</v>
+      </c>
+      <c r="U37" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -6534,8 +7080,14 @@
       <c r="N38" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="T38" t="s">
+        <v>212</v>
+      </c>
+      <c r="U38" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -6554,8 +7106,14 @@
       <c r="H39" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:16">
+      <c r="T39" t="s">
+        <v>213</v>
+      </c>
+      <c r="U39" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -6574,8 +7132,14 @@
       <c r="H40" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:16">
+      <c r="T40" t="s">
+        <v>214</v>
+      </c>
+      <c r="U40" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -6594,8 +7158,14 @@
       <c r="H41" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:16">
+      <c r="T41" t="s">
+        <v>215</v>
+      </c>
+      <c r="U41" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -6617,8 +7187,14 @@
       <c r="N42" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:16">
+      <c r="T42" t="s">
+        <v>216</v>
+      </c>
+      <c r="U42" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -6637,8 +7213,14 @@
       <c r="F43" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:16">
+      <c r="T43" t="s">
+        <v>217</v>
+      </c>
+      <c r="U43" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
       <c r="A44" t="s">
         <v>95</v>
       </c>
@@ -6660,8 +7242,14 @@
       <c r="O44" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:16">
+      <c r="T44" t="s">
+        <v>218</v>
+      </c>
+      <c r="U44" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -6683,8 +7271,14 @@
       <c r="O45" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:16">
+      <c r="T45" t="s">
+        <v>219</v>
+      </c>
+      <c r="U45" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21">
       <c r="A46" t="s">
         <v>98</v>
       </c>
@@ -6703,8 +7297,14 @@
       <c r="P46" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:16">
+      <c r="T46" t="s">
+        <v>220</v>
+      </c>
+      <c r="U46" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21">
       <c r="A47" t="s">
         <v>100</v>
       </c>
@@ -6723,8 +7323,14 @@
       <c r="P47" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:16">
+      <c r="T47" t="s">
+        <v>221</v>
+      </c>
+      <c r="U47" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
       <c r="A48" t="s">
         <v>136</v>
       </c>
@@ -6746,8 +7352,14 @@
       <c r="P48" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:19">
+      <c r="T48" t="s">
+        <v>222</v>
+      </c>
+      <c r="U48" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21">
       <c r="A49" t="s">
         <v>143</v>
       </c>
@@ -6772,8 +7384,14 @@
       <c r="R49" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="50" spans="1:19">
+      <c r="T49" t="s">
+        <v>223</v>
+      </c>
+      <c r="U49" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21">
       <c r="A50" t="s">
         <v>141</v>
       </c>
@@ -6795,8 +7413,14 @@
       <c r="R50" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="51" spans="1:19">
+      <c r="T50" t="s">
+        <v>224</v>
+      </c>
+      <c r="U50" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21">
       <c r="A51" s="3" t="s">
         <v>147</v>
       </c>
@@ -6824,8 +7448,14 @@
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
-    </row>
-    <row r="52" spans="1:19">
+      <c r="T51" t="s">
+        <v>225</v>
+      </c>
+      <c r="U51" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21">
       <c r="A52" s="3" t="s">
         <v>148</v>
       </c>
@@ -6856,8 +7486,14 @@
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
       <c r="S52" s="3"/>
-    </row>
-    <row r="53" spans="1:19">
+      <c r="T52" t="s">
+        <v>226</v>
+      </c>
+      <c r="U52" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -6873,8 +7509,14 @@
       <c r="F53" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:19">
+      <c r="T53" t="s">
+        <v>227</v>
+      </c>
+      <c r="U53" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21">
       <c r="A54" t="s">
         <v>159</v>
       </c>
@@ -6890,8 +7532,14 @@
       <c r="F54" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:19">
+      <c r="T54" t="s">
+        <v>228</v>
+      </c>
+      <c r="U54" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21">
       <c r="A55" t="s">
         <v>162</v>
       </c>
@@ -6912,6 +7560,12 @@
       </c>
       <c r="S55" t="s">
         <v>164</v>
+      </c>
+      <c r="T55" t="s">
+        <v>229</v>
+      </c>
+      <c r="U55" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed the labels and descriptions from some attributes
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33580" windowHeight="16060" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33580" windowHeight="20540" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="org_molgenis_test_TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="263">
   <si>
     <t>text</t>
   </si>
@@ -553,9 +553,6 @@
     <t>xstringhidden</t>
   </si>
   <si>
-    <t>TypeTest identifer attribute</t>
-  </si>
-  <si>
     <t>TypeTest boolean attribute</t>
   </si>
   <si>
@@ -565,9 +562,6 @@
     <t>TypeTest compound attribute</t>
   </si>
   <si>
-    <t>TypeTest compound int attribute</t>
-  </si>
-  <si>
     <t>TypeTestRef value attribute</t>
   </si>
   <si>
@@ -595,9 +589,6 @@
     <t>Typetest nillable date attribute</t>
   </si>
   <si>
-    <t>Typetest datetime attribute</t>
-  </si>
-  <si>
     <t>Typetest nillable datetime attribute</t>
   </si>
   <si>
@@ -619,9 +610,6 @@
     <t>Typetest nillable enum attribute</t>
   </si>
   <si>
-    <t>Typetest html attribute</t>
-  </si>
-  <si>
     <t>Typetest nillable html attribute</t>
   </si>
   <si>
@@ -634,9 +622,6 @@
     <t>Typetest int attribute</t>
   </si>
   <si>
-    <t>Typetest nillable int attribute</t>
-  </si>
-  <si>
     <t>Typetest int range attribute</t>
   </si>
   <si>
@@ -646,9 +631,6 @@
     <t>Typetest long attribute</t>
   </si>
   <si>
-    <t>Typetest nillable long attribute</t>
-  </si>
-  <si>
     <t>Typetest longrange attribute</t>
   </si>
   <si>
@@ -658,18 +640,12 @@
     <t>Typetest mref attribute</t>
   </si>
   <si>
-    <t>Typetest nillable mref attribute_value</t>
-  </si>
-  <si>
     <t>Typetest string attribute</t>
   </si>
   <si>
     <t>Typetest nillable string attribute</t>
   </si>
   <si>
-    <t>Typetest text attribute</t>
-  </si>
-  <si>
     <t>Typetest nillable text attribute</t>
   </si>
   <si>
@@ -685,9 +661,6 @@
     <t>Typetest nillable hidden string attribute</t>
   </si>
   <si>
-    <t>Typetest unique string attribute</t>
-  </si>
-  <si>
     <t>Typetest unique int attribute</t>
   </si>
   <si>
@@ -700,9 +673,6 @@
     <t>Typetest computed int attribute</t>
   </si>
   <si>
-    <t>Location Chromosome attribute</t>
-  </si>
-  <si>
     <t>Location Position attribute</t>
   </si>
   <si>
@@ -724,9 +694,6 @@
     <t>id label</t>
   </si>
   <si>
-    <t>xbool label</t>
-  </si>
-  <si>
     <t>xboolnillable label</t>
   </si>
   <si>
@@ -742,15 +709,6 @@
     <t>xcategorical_value label</t>
   </si>
   <si>
-    <t>xcategoricalnillable_value label</t>
-  </si>
-  <si>
-    <t>xcategoricalmref_value label</t>
-  </si>
-  <si>
-    <t>xcatmrefnillable_value label</t>
-  </si>
-  <si>
     <t>xdate label</t>
   </si>
   <si>
@@ -775,9 +733,6 @@
     <t>xemailnillable label</t>
   </si>
   <si>
-    <t>xenum label</t>
-  </si>
-  <si>
     <t>xenumnillable label</t>
   </si>
   <si>
@@ -817,12 +772,6 @@
     <t>xlongrangenillable label</t>
   </si>
   <si>
-    <t>xmref_value label</t>
-  </si>
-  <si>
-    <t>xmrefnillable_value label</t>
-  </si>
-  <si>
     <t>xstring label</t>
   </si>
   <si>
@@ -835,12 +784,6 @@
     <t>xtextnillable label</t>
   </si>
   <si>
-    <t>xxref_value label</t>
-  </si>
-  <si>
-    <t>xxrefnillable_value label</t>
-  </si>
-  <si>
     <t>xstring_hidden label</t>
   </si>
   <si>
@@ -851,9 +794,6 @@
   </si>
   <si>
     <t>xint_unique label</t>
-  </si>
-  <si>
-    <t>xxref_unique label</t>
   </si>
   <si>
     <t>xcomputedxref label</t>
@@ -5949,8 +5889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2:U55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6052,10 +5992,10 @@
         <v>1</v>
       </c>
       <c r="T2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="U2" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -6081,10 +6021,10 @@
         <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="U3" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -6106,11 +6046,8 @@
       <c r="M4" t="b">
         <v>1</v>
       </c>
-      <c r="T4" t="s">
-        <v>176</v>
-      </c>
       <c r="U4" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -6136,10 +6073,7 @@
         <v>1</v>
       </c>
       <c r="T5" t="s">
-        <v>177</v>
-      </c>
-      <c r="U5" t="s">
-        <v>233</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -6165,10 +6099,10 @@
         <v>1</v>
       </c>
       <c r="T6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="U6" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -6188,10 +6122,10 @@
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="U7" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -6219,11 +6153,8 @@
       <c r="Q8" t="s">
         <v>149</v>
       </c>
-      <c r="T8" t="s">
-        <v>180</v>
-      </c>
       <c r="U8" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -6252,10 +6183,10 @@
         <v>149</v>
       </c>
       <c r="T9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="U9" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -6281,10 +6212,10 @@
         <v>2</v>
       </c>
       <c r="T10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="U10" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -6310,10 +6241,7 @@
         <v>3</v>
       </c>
       <c r="T11" t="s">
-        <v>185</v>
-      </c>
-      <c r="U11" t="s">
-        <v>239</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -6342,10 +6270,7 @@
         <v>1</v>
       </c>
       <c r="T12" t="s">
-        <v>186</v>
-      </c>
-      <c r="U12" t="s">
-        <v>240</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -6371,10 +6296,7 @@
         <v>170</v>
       </c>
       <c r="T13" t="s">
-        <v>187</v>
-      </c>
-      <c r="U13" t="s">
-        <v>241</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -6400,10 +6322,10 @@
         <v>1</v>
       </c>
       <c r="T14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="U14" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -6426,10 +6348,10 @@
         <v>42095</v>
       </c>
       <c r="T15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="U15" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -6451,11 +6373,8 @@
       <c r="H16" t="s">
         <v>6</v>
       </c>
-      <c r="T16" t="s">
-        <v>190</v>
-      </c>
       <c r="U16" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -6481,10 +6400,10 @@
         <v>1</v>
       </c>
       <c r="T17" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="U17" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -6510,10 +6429,10 @@
         <v>1</v>
       </c>
       <c r="T18" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="U18" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -6536,10 +6455,10 @@
         <v>15.666</v>
       </c>
       <c r="T19" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="U19" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -6565,10 +6484,10 @@
         <v>1</v>
       </c>
       <c r="T20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="U20" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -6591,10 +6510,10 @@
         <v>7</v>
       </c>
       <c r="T21" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="U21" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -6623,10 +6542,7 @@
         <v>1</v>
       </c>
       <c r="T22" t="s">
-        <v>196</v>
-      </c>
-      <c r="U22" t="s">
-        <v>250</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -6652,10 +6568,10 @@
         <v>10</v>
       </c>
       <c r="T23" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="U23" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -6677,11 +6593,8 @@
       <c r="H24" t="s">
         <v>11</v>
       </c>
-      <c r="T24" t="s">
-        <v>198</v>
-      </c>
       <c r="U24" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -6707,10 +6620,10 @@
         <v>1</v>
       </c>
       <c r="T25" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="U25" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -6736,10 +6649,10 @@
         <v>1</v>
       </c>
       <c r="T26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="U26" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
     </row>
     <row r="27" spans="1:21">
@@ -6762,10 +6675,10 @@
         <v>174</v>
       </c>
       <c r="T27" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="U27" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -6791,10 +6704,10 @@
         <v>1</v>
       </c>
       <c r="T28" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="U28" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
     </row>
     <row r="29" spans="1:21">
@@ -6816,11 +6729,8 @@
       <c r="H29">
         <v>1</v>
       </c>
-      <c r="T29" t="s">
-        <v>203</v>
-      </c>
       <c r="U29" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -6846,10 +6756,10 @@
         <v>10</v>
       </c>
       <c r="T30" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="U30" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -6875,10 +6785,10 @@
         <v>0</v>
       </c>
       <c r="T31" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="U31" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
     </row>
     <row r="32" spans="1:21">
@@ -6901,10 +6811,10 @@
         <v>12342151234</v>
       </c>
       <c r="T32" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="U32" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:21">
@@ -6926,11 +6836,8 @@
       <c r="H33">
         <v>12342151234</v>
       </c>
-      <c r="T33" t="s">
-        <v>207</v>
-      </c>
       <c r="U33" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="34" spans="1:21">
@@ -6962,10 +6869,10 @@
         <v>1</v>
       </c>
       <c r="T34" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="U34" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" spans="1:21">
@@ -6997,10 +6904,10 @@
         <v>1</v>
       </c>
       <c r="T35" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="U35" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
     </row>
     <row r="36" spans="1:21">
@@ -7026,10 +6933,7 @@
         <v>1</v>
       </c>
       <c r="T36" t="s">
-        <v>210</v>
-      </c>
-      <c r="U36" t="s">
-        <v>264</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:21">
@@ -7051,12 +6955,6 @@
       <c r="F37" t="b">
         <v>1</v>
       </c>
-      <c r="T37" t="s">
-        <v>211</v>
-      </c>
-      <c r="U37" t="s">
-        <v>265</v>
-      </c>
     </row>
     <row r="38" spans="1:21">
       <c r="A38" t="s">
@@ -7081,10 +6979,10 @@
         <v>1</v>
       </c>
       <c r="T38" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="U38" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:21">
@@ -7107,10 +7005,10 @@
         <v>39</v>
       </c>
       <c r="T39" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="U39" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="40" spans="1:21">
@@ -7132,11 +7030,8 @@
       <c r="H40" t="s">
         <v>40</v>
       </c>
-      <c r="T40" t="s">
-        <v>214</v>
-      </c>
       <c r="U40" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
     </row>
     <row r="41" spans="1:21">
@@ -7159,10 +7054,10 @@
         <v>41</v>
       </c>
       <c r="T41" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="U41" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
     </row>
     <row r="42" spans="1:21">
@@ -7188,10 +7083,7 @@
         <v>1</v>
       </c>
       <c r="T42" t="s">
-        <v>216</v>
-      </c>
-      <c r="U42" t="s">
-        <v>270</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:21">
@@ -7214,10 +7106,7 @@
         <v>1</v>
       </c>
       <c r="T43" t="s">
-        <v>217</v>
-      </c>
-      <c r="U43" t="s">
-        <v>271</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:21">
@@ -7243,10 +7132,10 @@
         <v>0</v>
       </c>
       <c r="T44" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="U44" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
     </row>
     <row r="45" spans="1:21">
@@ -7272,10 +7161,10 @@
         <v>0</v>
       </c>
       <c r="T45" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="U45" t="s">
-        <v>273</v>
+        <v>254</v>
       </c>
     </row>
     <row r="46" spans="1:21">
@@ -7297,11 +7186,8 @@
       <c r="P46" t="b">
         <v>1</v>
       </c>
-      <c r="T46" t="s">
-        <v>220</v>
-      </c>
       <c r="U46" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
     </row>
     <row r="47" spans="1:21">
@@ -7324,10 +7210,10 @@
         <v>1</v>
       </c>
       <c r="T47" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="U47" t="s">
-        <v>275</v>
+        <v>256</v>
       </c>
     </row>
     <row r="48" spans="1:21">
@@ -7353,10 +7239,7 @@
         <v>1</v>
       </c>
       <c r="T48" t="s">
-        <v>222</v>
-      </c>
-      <c r="U48" t="s">
-        <v>276</v>
+        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -7385,10 +7268,10 @@
         <v>146</v>
       </c>
       <c r="T49" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="U49" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
     </row>
     <row r="50" spans="1:21">
@@ -7414,10 +7297,10 @@
         <v>29</v>
       </c>
       <c r="T50" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="U50" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
     </row>
     <row r="51" spans="1:21">
@@ -7448,11 +7331,8 @@
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
-      <c r="T51" t="s">
-        <v>225</v>
-      </c>
       <c r="U51" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52" spans="1:21">
@@ -7487,10 +7367,10 @@
       <c r="R52" s="3"/>
       <c r="S52" s="3"/>
       <c r="T52" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="U52" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
     </row>
     <row r="53" spans="1:21">
@@ -7510,10 +7390,10 @@
         <v>0</v>
       </c>
       <c r="T53" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="U53" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="54" spans="1:21">
@@ -7533,10 +7413,10 @@
         <v>1</v>
       </c>
       <c r="T54" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="U54" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
     </row>
     <row r="55" spans="1:21">
@@ -7562,15 +7442,14 @@
         <v>164</v>
       </c>
       <c r="T55" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="U55" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
updated test emx for row level security
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33580" windowHeight="20540" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="org_molgenis_test_TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="264">
   <si>
     <t>text</t>
   </si>
@@ -812,6 +812,9 @@
   </si>
   <si>
     <t>driverslicence label</t>
+  </si>
+  <si>
+    <t>rowLevelSecured</t>
   </si>
 </sst>
 </file>
@@ -5827,10 +5830,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5840,7 +5843,7 @@
     <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5853,8 +5856,11 @@
       <c r="D1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -5864,13 +5870,16 @@
       <c r="C2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -5889,7 +5898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add File type attribute to TypeTest
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33580" windowHeight="20540" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33580" windowHeight="20540"/>
   </bookViews>
   <sheets>
     <sheet name="org_molgenis_test_TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="266">
   <si>
     <t>text</t>
   </si>
@@ -812,6 +812,15 @@
   </si>
   <si>
     <t>driverslicence label</t>
+  </si>
+  <si>
+    <t>xfile</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>FileMeta</t>
   </si>
 </sst>
 </file>
@@ -867,9 +876,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -893,7 +903,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="18">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -909,6 +919,7 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1209,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR39"/>
+  <dimension ref="A1:AS39"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AW21" sqref="AW21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1245,7 +1256,7 @@
     <col min="42" max="42" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:45">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -1378,8 +1389,11 @@
       <c r="AR1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="2" spans="1:44">
+      <c r="AS1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1513,7 +1527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1647,7 +1661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1727,7 +1741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1861,7 +1875,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1995,7 +2009,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2072,7 +2086,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2203,7 +2217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2334,7 +2348,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2411,7 +2425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2542,7 +2556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:44">
+    <row r="12" spans="1:45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2673,7 +2687,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:44">
+    <row r="13" spans="1:45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2750,7 +2764,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:44">
+    <row r="14" spans="1:45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2881,7 +2895,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:44">
+    <row r="15" spans="1:45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3012,7 +3026,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
+    <row r="16" spans="1:45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5887,10 +5901,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U55"/>
+  <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="T49" sqref="T49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7244,110 +7258,98 @@
     </row>
     <row r="49" spans="1:21">
       <c r="A49" t="s">
-        <v>143</v>
+        <v>263</v>
       </c>
       <c r="B49" t="s">
         <v>167</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>264</v>
       </c>
       <c r="D49" t="s">
-        <v>145</v>
+        <v>265</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
       </c>
       <c r="F49" t="b">
         <v>1</v>
-      </c>
-      <c r="M49" t="b">
-        <v>1</v>
-      </c>
-      <c r="R49" t="s">
-        <v>146</v>
-      </c>
-      <c r="T49" t="s">
-        <v>214</v>
-      </c>
-      <c r="U49" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="50" spans="1:21">
       <c r="A50" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B50" t="s">
         <v>167</v>
       </c>
       <c r="C50" t="s">
+        <v>78</v>
+      </c>
+      <c r="D50" t="s">
+        <v>145</v>
+      </c>
+      <c r="E50" t="b">
+        <v>0</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+      <c r="M50" t="b">
+        <v>1</v>
+      </c>
+      <c r="R50" t="s">
+        <v>146</v>
+      </c>
+      <c r="T50" t="s">
+        <v>214</v>
+      </c>
+      <c r="U50" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21">
+      <c r="A51" t="s">
+        <v>141</v>
+      </c>
+      <c r="B51" t="s">
+        <v>167</v>
+      </c>
+      <c r="C51" t="s">
         <v>67</v>
       </c>
-      <c r="E50" t="b">
-        <v>0</v>
-      </c>
-      <c r="F50" t="b">
-        <v>1</v>
-      </c>
-      <c r="M50" t="b">
-        <v>1</v>
-      </c>
-      <c r="R50" t="s">
+      <c r="E51" t="b">
+        <v>0</v>
+      </c>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
+      <c r="M51" t="b">
+        <v>1</v>
+      </c>
+      <c r="R51" t="s">
         <v>29</v>
       </c>
-      <c r="T50" t="s">
+      <c r="T51" t="s">
         <v>215</v>
       </c>
-      <c r="U50" t="s">
+      <c r="U51" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21">
-      <c r="A51" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F51" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
-      <c r="R51" s="3"/>
-      <c r="U51" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="52" spans="1:21">
       <c r="A52" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>145</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52" s="3" t="b">
         <v>0</v>
@@ -7357,99 +7359,132 @@
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
-      <c r="L52" s="3" t="b">
-        <v>1</v>
-      </c>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
-      <c r="S52" s="3"/>
-      <c r="T52" t="s">
+      <c r="U52" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21">
+      <c r="A53" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3"/>
+      <c r="T53" t="s">
         <v>216</v>
       </c>
-      <c r="U52" t="s">
+      <c r="U53" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21">
-      <c r="A53" t="s">
-        <v>60</v>
-      </c>
-      <c r="B53" t="s">
-        <v>160</v>
-      </c>
-      <c r="C53" t="s">
-        <v>66</v>
-      </c>
-      <c r="E53" t="s">
-        <v>161</v>
-      </c>
-      <c r="F53" t="b">
-        <v>0</v>
-      </c>
-      <c r="T53" t="s">
-        <v>217</v>
-      </c>
-      <c r="U53" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="54" spans="1:21">
       <c r="A54" t="s">
-        <v>159</v>
+        <v>60</v>
       </c>
       <c r="B54" t="s">
         <v>160</v>
       </c>
       <c r="C54" t="s">
-        <v>67</v>
-      </c>
-      <c r="E54" t="b">
-        <v>0</v>
+        <v>66</v>
+      </c>
+      <c r="E54" t="s">
+        <v>161</v>
       </c>
       <c r="F54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T54" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U54" t="s">
-        <v>261</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:21">
       <c r="A55" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B55" t="s">
         <v>160</v>
       </c>
       <c r="C55" t="s">
+        <v>67</v>
+      </c>
+      <c r="E55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
+      <c r="T55" t="s">
+        <v>218</v>
+      </c>
+      <c r="U55" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21">
+      <c r="A56" t="s">
+        <v>162</v>
+      </c>
+      <c r="B56" t="s">
+        <v>160</v>
+      </c>
+      <c r="C56" t="s">
         <v>68</v>
       </c>
-      <c r="E55" t="b">
-        <v>0</v>
-      </c>
-      <c r="F55" t="b">
-        <v>1</v>
-      </c>
-      <c r="O55" s="3" t="s">
+      <c r="E56" t="b">
+        <v>0</v>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+      <c r="O56" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="S55" t="s">
+      <c r="S56" t="s">
         <v>164</v>
       </c>
-      <c r="T55" t="s">
+      <c r="T56" t="s">
         <v>219</v>
       </c>
-      <c r="U55" t="s">
+      <c r="U56" t="s">
         <v>262</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added xfile attribute to the EMX all datatypes
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="265">
   <si>
     <t>text</t>
   </si>
@@ -812,6 +812,12 @@
   </si>
   <si>
     <t>driverslicence label</t>
+  </si>
+  <si>
+    <t>xfile</t>
+  </si>
+  <si>
+    <t>file</t>
   </si>
 </sst>
 </file>
@@ -867,9 +873,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -893,7 +901,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -909,6 +917,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1209,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR39"/>
+  <dimension ref="A1:AS39"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AT26" sqref="AT26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1245,7 +1255,7 @@
     <col min="42" max="42" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:45">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -1378,8 +1388,11 @@
       <c r="AR1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="2" spans="1:44">
+      <c r="AS1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1513,7 +1526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1647,7 +1660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1727,7 +1740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1861,7 +1874,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1995,7 +2008,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2072,7 +2085,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2203,7 +2216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2334,7 +2347,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2411,7 +2424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2542,7 +2555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:44">
+    <row r="12" spans="1:45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2673,7 +2686,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:44">
+    <row r="13" spans="1:45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2750,7 +2763,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:44">
+    <row r="14" spans="1:45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2881,7 +2894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:44">
+    <row r="15" spans="1:45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3012,7 +3025,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
+    <row r="16" spans="1:45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5887,10 +5900,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U55"/>
+  <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7244,110 +7257,95 @@
     </row>
     <row r="49" spans="1:21">
       <c r="A49" t="s">
-        <v>143</v>
+        <v>263</v>
       </c>
       <c r="B49" t="s">
         <v>167</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
-      </c>
-      <c r="D49" t="s">
-        <v>145</v>
+        <v>264</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
       </c>
       <c r="F49" t="b">
         <v>1</v>
-      </c>
-      <c r="M49" t="b">
-        <v>1</v>
-      </c>
-      <c r="R49" t="s">
-        <v>146</v>
-      </c>
-      <c r="T49" t="s">
-        <v>214</v>
-      </c>
-      <c r="U49" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="50" spans="1:21">
       <c r="A50" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B50" t="s">
         <v>167</v>
       </c>
       <c r="C50" t="s">
+        <v>78</v>
+      </c>
+      <c r="D50" t="s">
+        <v>145</v>
+      </c>
+      <c r="E50" t="b">
+        <v>0</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+      <c r="M50" t="b">
+        <v>1</v>
+      </c>
+      <c r="R50" t="s">
+        <v>146</v>
+      </c>
+      <c r="T50" t="s">
+        <v>214</v>
+      </c>
+      <c r="U50" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21">
+      <c r="A51" t="s">
+        <v>141</v>
+      </c>
+      <c r="B51" t="s">
+        <v>167</v>
+      </c>
+      <c r="C51" t="s">
         <v>67</v>
       </c>
-      <c r="E50" t="b">
-        <v>0</v>
-      </c>
-      <c r="F50" t="b">
-        <v>1</v>
-      </c>
-      <c r="M50" t="b">
-        <v>1</v>
-      </c>
-      <c r="R50" t="s">
+      <c r="E51" t="b">
+        <v>0</v>
+      </c>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
+      <c r="M51" t="b">
+        <v>1</v>
+      </c>
+      <c r="R51" t="s">
         <v>29</v>
       </c>
-      <c r="T50" t="s">
+      <c r="T51" t="s">
         <v>215</v>
       </c>
-      <c r="U50" t="s">
+      <c r="U51" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21">
-      <c r="A51" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F51" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
-      <c r="R51" s="3"/>
-      <c r="U51" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="52" spans="1:21">
       <c r="A52" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>145</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52" s="3" t="b">
         <v>0</v>
@@ -7357,99 +7355,132 @@
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
-      <c r="L52" s="3" t="b">
-        <v>1</v>
-      </c>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
-      <c r="S52" s="3"/>
-      <c r="T52" t="s">
+      <c r="U52" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21">
+      <c r="A53" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3"/>
+      <c r="T53" t="s">
         <v>216</v>
       </c>
-      <c r="U52" t="s">
+      <c r="U53" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21">
-      <c r="A53" t="s">
-        <v>60</v>
-      </c>
-      <c r="B53" t="s">
-        <v>160</v>
-      </c>
-      <c r="C53" t="s">
-        <v>66</v>
-      </c>
-      <c r="E53" t="s">
-        <v>161</v>
-      </c>
-      <c r="F53" t="b">
-        <v>0</v>
-      </c>
-      <c r="T53" t="s">
-        <v>217</v>
-      </c>
-      <c r="U53" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="54" spans="1:21">
       <c r="A54" t="s">
-        <v>159</v>
+        <v>60</v>
       </c>
       <c r="B54" t="s">
         <v>160</v>
       </c>
       <c r="C54" t="s">
-        <v>67</v>
-      </c>
-      <c r="E54" t="b">
-        <v>0</v>
+        <v>66</v>
+      </c>
+      <c r="E54" t="s">
+        <v>161</v>
       </c>
       <c r="F54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T54" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U54" t="s">
-        <v>261</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:21">
       <c r="A55" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B55" t="s">
         <v>160</v>
       </c>
       <c r="C55" t="s">
+        <v>67</v>
+      </c>
+      <c r="E55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
+      <c r="T55" t="s">
+        <v>218</v>
+      </c>
+      <c r="U55" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21">
+      <c r="A56" t="s">
+        <v>162</v>
+      </c>
+      <c r="B56" t="s">
+        <v>160</v>
+      </c>
+      <c r="C56" t="s">
         <v>68</v>
       </c>
-      <c r="E55" t="b">
-        <v>0</v>
-      </c>
-      <c r="F55" t="b">
-        <v>1</v>
-      </c>
-      <c r="O55" s="3" t="s">
+      <c r="E56" t="b">
+        <v>0</v>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+      <c r="O56" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="S55" t="s">
+      <c r="S56" t="s">
         <v>164</v>
       </c>
-      <c r="T55" t="s">
+      <c r="T56" t="s">
         <v>219</v>
       </c>
-      <c r="U55" t="s">
+      <c r="U56" t="s">
         <v>262</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
AttributeMetaDataMetaData -> AttributeMetadata aggregateable -> aggregatable
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33580" windowHeight="20540" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="org_molgenis_test_TypeTest" sheetId="1" r:id="rId1"/>
@@ -304,9 +304,6 @@
     <t>readOnly</t>
   </si>
   <si>
-    <t>aggregateable</t>
-  </si>
-  <si>
     <t>visible</t>
   </si>
   <si>
@@ -818,6 +815,9 @@
   </si>
   <si>
     <t>file</t>
+  </si>
+  <si>
+    <t>aggregatable</t>
   </si>
 </sst>
 </file>
@@ -1266,10 +1266,10 @@
         <v>45</v>
       </c>
       <c r="D1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" t="s">
         <v>151</v>
-      </c>
-      <c r="E1" t="s">
-        <v>152</v>
       </c>
       <c r="F1" t="s">
         <v>46</v>
@@ -1278,10 +1278,10 @@
         <v>19</v>
       </c>
       <c r="H1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I1" t="s">
         <v>156</v>
-      </c>
-      <c r="I1" t="s">
-        <v>157</v>
       </c>
       <c r="J1" t="s">
         <v>20</v>
@@ -1374,22 +1374,22 @@
         <v>43</v>
       </c>
       <c r="AN1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AO1" t="s">
         <v>95</v>
       </c>
-      <c r="AO1" t="s">
-        <v>96</v>
-      </c>
       <c r="AP1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AQ1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AR1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AS1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:45">
@@ -1406,7 +1406,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -1511,10 +1511,10 @@
         <v>2</v>
       </c>
       <c r="AN2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP2" t="s">
         <v>16</v>
@@ -1540,7 +1540,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
@@ -1645,10 +1645,10 @@
         <v>3</v>
       </c>
       <c r="AN3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP3" t="s">
         <v>17</v>
@@ -1671,7 +1671,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
@@ -1725,10 +1725,10 @@
         <v>4</v>
       </c>
       <c r="AN4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP4" t="s">
         <v>18</v>
@@ -1754,7 +1754,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F5" t="s">
         <v>2</v>
@@ -1859,13 +1859,13 @@
         <v>2</v>
       </c>
       <c r="AN5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AQ5">
         <v>4</v>
@@ -1888,7 +1888,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
@@ -1993,13 +1993,13 @@
         <v>3</v>
       </c>
       <c r="AN6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AQ6">
         <v>5</v>
@@ -2019,7 +2019,7 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F7" t="s">
         <v>4</v>
@@ -2073,13 +2073,13 @@
         <v>4</v>
       </c>
       <c r="AN7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AQ7">
         <v>6</v>
@@ -2099,7 +2099,7 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F8" t="s">
         <v>2</v>
@@ -2204,13 +2204,13 @@
         <v>2</v>
       </c>
       <c r="AN8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AQ8">
         <v>7</v>
@@ -2230,7 +2230,7 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F9" t="s">
         <v>3</v>
@@ -2335,13 +2335,13 @@
         <v>3</v>
       </c>
       <c r="AN9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AQ9">
         <v>8</v>
@@ -2358,7 +2358,7 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F10" t="s">
         <v>4</v>
@@ -2412,13 +2412,13 @@
         <v>4</v>
       </c>
       <c r="AN10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AQ10">
         <v>9</v>
@@ -2438,7 +2438,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F11" t="s">
         <v>2</v>
@@ -2543,13 +2543,13 @@
         <v>2</v>
       </c>
       <c r="AN11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AQ11">
         <v>10</v>
@@ -2569,7 +2569,7 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F12" t="s">
         <v>3</v>
@@ -2674,13 +2674,13 @@
         <v>3</v>
       </c>
       <c r="AN12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AQ12">
         <v>11</v>
@@ -2697,7 +2697,7 @@
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F13" t="s">
         <v>4</v>
@@ -2751,13 +2751,13 @@
         <v>4</v>
       </c>
       <c r="AN13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AQ13">
         <v>12</v>
@@ -2777,7 +2777,7 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F14" t="s">
         <v>2</v>
@@ -2882,13 +2882,13 @@
         <v>2</v>
       </c>
       <c r="AN14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AQ14">
         <v>13</v>
@@ -2908,7 +2908,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F15" t="s">
         <v>3</v>
@@ -3013,13 +3013,13 @@
         <v>3</v>
       </c>
       <c r="AN15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AQ15">
         <v>14</v>
@@ -3036,7 +3036,7 @@
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F16" t="s">
         <v>4</v>
@@ -3090,13 +3090,13 @@
         <v>4</v>
       </c>
       <c r="AN16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AQ16">
         <v>15</v>
@@ -3113,7 +3113,7 @@
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F17" t="s">
         <v>4</v>
@@ -3167,13 +3167,13 @@
         <v>4</v>
       </c>
       <c r="AN17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AQ17">
         <v>16</v>
@@ -3193,7 +3193,7 @@
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F18" t="s">
         <v>2</v>
@@ -3298,13 +3298,13 @@
         <v>2</v>
       </c>
       <c r="AN18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AQ18">
         <v>17</v>
@@ -3324,7 +3324,7 @@
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F19" t="s">
         <v>3</v>
@@ -3429,13 +3429,13 @@
         <v>3</v>
       </c>
       <c r="AN19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AQ19">
         <v>18</v>
@@ -3452,7 +3452,7 @@
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F20" t="s">
         <v>4</v>
@@ -3506,13 +3506,13 @@
         <v>4</v>
       </c>
       <c r="AN20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AQ20">
         <v>19</v>
@@ -3532,7 +3532,7 @@
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F21" t="s">
         <v>2</v>
@@ -3637,13 +3637,13 @@
         <v>2</v>
       </c>
       <c r="AN21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AQ21">
         <v>20</v>
@@ -3663,7 +3663,7 @@
         <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F22" t="s">
         <v>3</v>
@@ -3768,10 +3768,10 @@
         <v>3</v>
       </c>
       <c r="AN22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AQ22">
         <v>21</v>
@@ -3788,7 +3788,7 @@
         <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F23" t="s">
         <v>4</v>
@@ -3842,10 +3842,10 @@
         <v>4</v>
       </c>
       <c r="AN23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AQ23">
         <v>22</v>
@@ -3865,7 +3865,7 @@
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F24" t="s">
         <v>2</v>
@@ -3970,10 +3970,10 @@
         <v>2</v>
       </c>
       <c r="AN24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AQ24">
         <v>23</v>
@@ -3993,7 +3993,7 @@
         <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F25" t="s">
         <v>3</v>
@@ -4098,10 +4098,10 @@
         <v>3</v>
       </c>
       <c r="AN25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AQ25">
         <v>24</v>
@@ -4118,7 +4118,7 @@
         <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F26" t="s">
         <v>4</v>
@@ -4172,10 +4172,10 @@
         <v>4</v>
       </c>
       <c r="AN26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AQ26">
         <v>25</v>
@@ -4195,7 +4195,7 @@
         <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F27" t="s">
         <v>2</v>
@@ -4300,10 +4300,10 @@
         <v>2</v>
       </c>
       <c r="AN27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AQ27">
         <v>26</v>
@@ -4323,7 +4323,7 @@
         <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F28" t="s">
         <v>3</v>
@@ -4428,10 +4428,10 @@
         <v>3</v>
       </c>
       <c r="AN28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AQ28">
         <v>27</v>
@@ -4448,7 +4448,7 @@
         <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F29" t="s">
         <v>4</v>
@@ -4502,10 +4502,10 @@
         <v>4</v>
       </c>
       <c r="AN29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AQ29">
         <v>28</v>
@@ -4525,7 +4525,7 @@
         <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F30" t="s">
         <v>2</v>
@@ -4630,10 +4630,10 @@
         <v>2</v>
       </c>
       <c r="AN30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AQ30">
         <v>29</v>
@@ -4653,7 +4653,7 @@
         <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F31" t="s">
         <v>3</v>
@@ -4758,10 +4758,10 @@
         <v>3</v>
       </c>
       <c r="AN31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AQ31">
         <v>30</v>
@@ -4778,7 +4778,7 @@
         <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F32" t="s">
         <v>4</v>
@@ -4832,10 +4832,10 @@
         <v>4</v>
       </c>
       <c r="AN32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AQ32">
         <v>31</v>
@@ -4855,7 +4855,7 @@
         <v>32</v>
       </c>
       <c r="E33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F33" t="s">
         <v>2</v>
@@ -4960,10 +4960,10 @@
         <v>2</v>
       </c>
       <c r="AN33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AQ33">
         <v>32</v>
@@ -4983,7 +4983,7 @@
         <v>33</v>
       </c>
       <c r="E34" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F34" t="s">
         <v>3</v>
@@ -5088,10 +5088,10 @@
         <v>3</v>
       </c>
       <c r="AN34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AQ34">
         <v>33</v>
@@ -5108,7 +5108,7 @@
         <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F35" t="s">
         <v>4</v>
@@ -5162,10 +5162,10 @@
         <v>4</v>
       </c>
       <c r="AN35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AQ35">
         <v>34</v>
@@ -5182,7 +5182,7 @@
         <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F36" t="s">
         <v>4</v>
@@ -5236,10 +5236,10 @@
         <v>4</v>
       </c>
       <c r="AN36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AQ36">
         <v>35</v>
@@ -5259,7 +5259,7 @@
         <v>36</v>
       </c>
       <c r="E37" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F37" t="s">
         <v>2</v>
@@ -5364,10 +5364,10 @@
         <v>2</v>
       </c>
       <c r="AN37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AQ37">
         <v>36</v>
@@ -5387,7 +5387,7 @@
         <v>37</v>
       </c>
       <c r="E38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F38" t="s">
         <v>3</v>
@@ -5492,10 +5492,10 @@
         <v>3</v>
       </c>
       <c r="AN38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AQ38">
         <v>37</v>
@@ -5512,7 +5512,7 @@
         <v>38</v>
       </c>
       <c r="E39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F39" t="s">
         <v>4</v>
@@ -5566,10 +5566,10 @@
         <v>4</v>
       </c>
       <c r="AN39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AQ39">
         <v>38</v>
@@ -5801,31 +5801,31 @@
         <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -5858,13 +5858,13 @@
         <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C1" t="s">
         <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5872,7 +5872,7 @@
         <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>
@@ -5885,7 +5885,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -5903,7 +5903,7 @@
   <dimension ref="A1:U56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5943,7 +5943,7 @@
         <v>79</v>
       </c>
       <c r="H1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I1" t="s">
         <v>82</v>
@@ -5961,22 +5961,22 @@
         <v>92</v>
       </c>
       <c r="N1" t="s">
+        <v>264</v>
+      </c>
+      <c r="O1" t="s">
         <v>93</v>
       </c>
-      <c r="O1" t="s">
-        <v>94</v>
-      </c>
       <c r="P1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="T1" t="s">
         <v>56</v>
@@ -6005,10 +6005,10 @@
         <v>1</v>
       </c>
       <c r="T2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="U2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -6034,10 +6034,10 @@
         <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="U3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -6045,7 +6045,7 @@
         <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C4" t="s">
         <v>67</v>
@@ -6060,7 +6060,7 @@
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -6068,7 +6068,7 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
         <v>68</v>
@@ -6086,7 +6086,7 @@
         <v>1</v>
       </c>
       <c r="T5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -6094,7 +6094,7 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" t="s">
         <v>68</v>
@@ -6112,22 +6112,22 @@
         <v>1</v>
       </c>
       <c r="T6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="U6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" t="s">
         <v>149</v>
       </c>
-      <c r="B7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C7" t="s">
-        <v>150</v>
-      </c>
       <c r="E7" t="b">
         <v>0</v>
       </c>
@@ -6135,18 +6135,18 @@
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="U7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C8" t="s">
         <v>67</v>
@@ -6164,18 +6164,18 @@
         <v>1</v>
       </c>
       <c r="Q8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="U8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C9" t="s">
         <v>66</v>
@@ -6187,19 +6187,19 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N9" t="b">
         <v>1</v>
       </c>
       <c r="Q9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="U9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -6207,7 +6207,7 @@
         <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C10" t="s">
         <v>69</v>
@@ -6225,10 +6225,10 @@
         <v>2</v>
       </c>
       <c r="T10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="U10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -6236,7 +6236,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C11" t="s">
         <v>69</v>
@@ -6254,18 +6254,18 @@
         <v>3</v>
       </c>
       <c r="T11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D12" t="s">
         <v>59</v>
@@ -6277,24 +6277,24 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N12" t="b">
         <v>1</v>
       </c>
       <c r="T12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D13" t="s">
         <v>59</v>
@@ -6306,10 +6306,10 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -6317,7 +6317,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C14" t="s">
         <v>70</v>
@@ -6335,10 +6335,10 @@
         <v>1</v>
       </c>
       <c r="T14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -6346,7 +6346,7 @@
         <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C15" t="s">
         <v>70</v>
@@ -6361,10 +6361,10 @@
         <v>42095</v>
       </c>
       <c r="T15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -6372,7 +6372,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C16" t="s">
         <v>71</v>
@@ -6387,7 +6387,7 @@
         <v>6</v>
       </c>
       <c r="U16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -6395,7 +6395,7 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C17" t="s">
         <v>71</v>
@@ -6413,10 +6413,10 @@
         <v>1</v>
       </c>
       <c r="T17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -6424,7 +6424,7 @@
         <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C18" t="s">
         <v>72</v>
@@ -6442,10 +6442,10 @@
         <v>1</v>
       </c>
       <c r="T18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="U18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -6453,7 +6453,7 @@
         <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C19" t="s">
         <v>72</v>
@@ -6468,10 +6468,10 @@
         <v>15.666</v>
       </c>
       <c r="T19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="U19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -6479,7 +6479,7 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C20" t="s">
         <v>73</v>
@@ -6491,16 +6491,16 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N20" t="b">
         <v>1</v>
       </c>
       <c r="T20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="U20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -6508,7 +6508,7 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C21" t="s">
         <v>73</v>
@@ -6523,10 +6523,10 @@
         <v>7</v>
       </c>
       <c r="T21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="U21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -6534,7 +6534,7 @@
         <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C22" t="s">
         <v>80</v>
@@ -6555,7 +6555,7 @@
         <v>1</v>
       </c>
       <c r="T22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -6563,7 +6563,7 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C23" t="s">
         <v>80</v>
@@ -6581,10 +6581,10 @@
         <v>10</v>
       </c>
       <c r="T23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="U23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -6592,7 +6592,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C24" t="s">
         <v>74</v>
@@ -6607,7 +6607,7 @@
         <v>11</v>
       </c>
       <c r="U24" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -6615,7 +6615,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C25" t="s">
         <v>74</v>
@@ -6627,16 +6627,16 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N25" t="b">
         <v>1</v>
       </c>
       <c r="T25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="U25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -6644,7 +6644,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C26" t="s">
         <v>75</v>
@@ -6656,16 +6656,16 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N26" t="b">
         <v>1</v>
       </c>
       <c r="T26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="U26" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="27" spans="1:21">
@@ -6673,7 +6673,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C27" t="s">
         <v>75</v>
@@ -6685,13 +6685,13 @@
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="U27" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -6699,7 +6699,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C28" t="s">
         <v>67</v>
@@ -6717,10 +6717,10 @@
         <v>1</v>
       </c>
       <c r="T28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="U28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="29" spans="1:21">
@@ -6728,7 +6728,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C29" t="s">
         <v>67</v>
@@ -6743,7 +6743,7 @@
         <v>1</v>
       </c>
       <c r="U29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -6751,7 +6751,7 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C30" t="s">
         <v>67</v>
@@ -6769,10 +6769,10 @@
         <v>10</v>
       </c>
       <c r="T30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="U30" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -6780,7 +6780,7 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C31" t="s">
         <v>67</v>
@@ -6798,10 +6798,10 @@
         <v>0</v>
       </c>
       <c r="T31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="U31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:21">
@@ -6809,7 +6809,7 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C32" t="s">
         <v>76</v>
@@ -6824,10 +6824,10 @@
         <v>12342151234</v>
       </c>
       <c r="T32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U32" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="1:21">
@@ -6835,7 +6835,7 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C33" t="s">
         <v>76</v>
@@ -6850,7 +6850,7 @@
         <v>12342151234</v>
       </c>
       <c r="U33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:21">
@@ -6858,7 +6858,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C34" t="s">
         <v>76</v>
@@ -6882,10 +6882,10 @@
         <v>1</v>
       </c>
       <c r="T34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U34" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="35" spans="1:21">
@@ -6893,7 +6893,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C35" t="s">
         <v>76</v>
@@ -6917,10 +6917,10 @@
         <v>1</v>
       </c>
       <c r="T35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U35" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="36" spans="1:21">
@@ -6928,7 +6928,7 @@
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C36" t="s">
         <v>77</v>
@@ -6946,7 +6946,7 @@
         <v>1</v>
       </c>
       <c r="T36" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="1:21">
@@ -6954,7 +6954,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C37" t="s">
         <v>77</v>
@@ -6974,7 +6974,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C38" t="s">
         <v>66</v>
@@ -6992,10 +6992,10 @@
         <v>1</v>
       </c>
       <c r="T38" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="U38" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="39" spans="1:21">
@@ -7003,7 +7003,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C39" t="s">
         <v>66</v>
@@ -7018,10 +7018,10 @@
         <v>39</v>
       </c>
       <c r="T39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="U39" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="40" spans="1:21">
@@ -7029,7 +7029,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
@@ -7044,7 +7044,7 @@
         <v>40</v>
       </c>
       <c r="U40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="41" spans="1:21">
@@ -7052,7 +7052,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
@@ -7067,10 +7067,10 @@
         <v>41</v>
       </c>
       <c r="T41" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="U41" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:21">
@@ -7078,7 +7078,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C42" t="s">
         <v>78</v>
@@ -7096,7 +7096,7 @@
         <v>1</v>
       </c>
       <c r="T42" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" spans="1:21">
@@ -7104,7 +7104,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C43" t="s">
         <v>78</v>
@@ -7119,15 +7119,15 @@
         <v>1</v>
       </c>
       <c r="T43" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="44" spans="1:21">
       <c r="A44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C44" t="s">
         <v>66</v>
@@ -7145,18 +7145,18 @@
         <v>0</v>
       </c>
       <c r="T44" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="U44" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="45" spans="1:21">
       <c r="A45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B45" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C45" t="s">
         <v>66</v>
@@ -7168,24 +7168,24 @@
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O45" t="b">
         <v>0</v>
       </c>
       <c r="T45" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="U45" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="46" spans="1:21">
       <c r="A46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C46" t="s">
         <v>66</v>
@@ -7200,15 +7200,15 @@
         <v>1</v>
       </c>
       <c r="U46" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="47" spans="1:21">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C47" t="s">
         <v>67</v>
@@ -7223,18 +7223,18 @@
         <v>1</v>
       </c>
       <c r="T47" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="U47" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="48" spans="1:21">
       <c r="A48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C48" t="s">
         <v>78</v>
@@ -7252,18 +7252,18 @@
         <v>1</v>
       </c>
       <c r="T48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="49" spans="1:21">
       <c r="A49" t="s">
+        <v>262</v>
+      </c>
+      <c r="B49" t="s">
+        <v>166</v>
+      </c>
+      <c r="C49" t="s">
         <v>263</v>
-      </c>
-      <c r="B49" t="s">
-        <v>167</v>
-      </c>
-      <c r="C49" t="s">
-        <v>264</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -7274,42 +7274,42 @@
     </row>
     <row r="50" spans="1:21">
       <c r="A50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B50" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C50" t="s">
         <v>78</v>
       </c>
       <c r="D50" t="s">
+        <v>144</v>
+      </c>
+      <c r="E50" t="b">
+        <v>0</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+      <c r="M50" t="b">
+        <v>1</v>
+      </c>
+      <c r="R50" t="s">
         <v>145</v>
       </c>
-      <c r="E50" t="b">
-        <v>0</v>
-      </c>
-      <c r="F50" t="b">
-        <v>1</v>
-      </c>
-      <c r="M50" t="b">
-        <v>1</v>
-      </c>
-      <c r="R50" t="s">
-        <v>146</v>
-      </c>
       <c r="T50" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="U50" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="51" spans="1:21">
       <c r="A51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C51" t="s">
         <v>67</v>
@@ -7327,18 +7327,18 @@
         <v>29</v>
       </c>
       <c r="T51" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="U51" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="52" spans="1:21">
       <c r="A52" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>66</v>
@@ -7362,15 +7362,15 @@
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
       <c r="U52" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="53" spans="1:21">
       <c r="A53" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>67</v>
@@ -7397,10 +7397,10 @@
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
       <c r="T53" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="U53" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="54" spans="1:21">
@@ -7408,30 +7408,30 @@
         <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C54" t="s">
         <v>66</v>
       </c>
       <c r="E54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F54" t="b">
         <v>0</v>
       </c>
       <c r="T54" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="U54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="1:21">
       <c r="A55" t="s">
+        <v>158</v>
+      </c>
+      <c r="B55" t="s">
         <v>159</v>
-      </c>
-      <c r="B55" t="s">
-        <v>160</v>
       </c>
       <c r="C55" t="s">
         <v>67</v>
@@ -7443,18 +7443,18 @@
         <v>1</v>
       </c>
       <c r="T55" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U55" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="56" spans="1:21">
       <c r="A56" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C56" t="s">
         <v>68</v>
@@ -7466,16 +7466,16 @@
         <v>1</v>
       </c>
       <c r="O56" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="S56" t="s">
         <v>163</v>
       </c>
-      <c r="S56" t="s">
-        <v>164</v>
-      </c>
       <c r="T56" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U56" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix emx_all_datatypes aggregatable to isAggregatable
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" activeTab="4"/>
@@ -817,7 +817,7 @@
     <t>file</t>
   </si>
   <si>
-    <t>aggregatable</t>
+    <t>isAggregatable</t>
   </si>
 </sst>
 </file>
@@ -7480,7 +7480,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Revert EMX changes. Add mapping between internal model and EMX
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="14600" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="org_molgenis_test_TypeTest" sheetId="1" r:id="rId1"/>
@@ -817,7 +817,7 @@
     <t>file</t>
   </si>
   <si>
-    <t>isAggregatable</t>
+    <t>aggregateable</t>
   </si>
 </sst>
 </file>
@@ -5903,7 +5903,7 @@
   <dimension ref="A1:U56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
fix emx + remove unique validation check + fix missing emailvalidator
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="14600" activeTab="4"/>
+    <workbookView xWindow="-38400" yWindow="1360" windowWidth="25600" windowHeight="15460" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="org_molgenis_test_TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="263">
   <si>
     <t>text</t>
   </si>
@@ -527,12 +527,6 @@
   </si>
   <si>
     <t>defaultValue</t>
-  </si>
-  <si>
-    <t>ref1,ref2</t>
-  </si>
-  <si>
-    <t>ref1,ref3</t>
   </si>
   <si>
     <t>test@x.y.z</t>
@@ -1389,7 +1383,7 @@
         <v>135</v>
       </c>
       <c r="AS1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:45">
@@ -5902,8 +5896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5961,7 +5955,7 @@
         <v>92</v>
       </c>
       <c r="N1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="O1" t="s">
         <v>93</v>
@@ -6005,10 +5999,10 @@
         <v>1</v>
       </c>
       <c r="T2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="U2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -6034,10 +6028,10 @@
         <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -6060,7 +6054,7 @@
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -6086,7 +6080,7 @@
         <v>1</v>
       </c>
       <c r="T5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -6112,10 +6106,10 @@
         <v>1</v>
       </c>
       <c r="T6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="U6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -6135,10 +6129,10 @@
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="U7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -6167,7 +6161,7 @@
         <v>148</v>
       </c>
       <c r="U8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -6196,10 +6190,10 @@
         <v>148</v>
       </c>
       <c r="T9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="U9" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -6221,14 +6215,11 @@
       <c r="F10" t="b">
         <v>0</v>
       </c>
-      <c r="H10" t="s">
-        <v>2</v>
-      </c>
       <c r="T10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="U10" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -6250,11 +6241,8 @@
       <c r="F11" t="b">
         <v>1</v>
       </c>
-      <c r="H11" t="s">
-        <v>3</v>
-      </c>
       <c r="T11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -6276,14 +6264,11 @@
       <c r="F12" t="b">
         <v>0</v>
       </c>
-      <c r="H12" t="s">
-        <v>168</v>
-      </c>
       <c r="N12" t="b">
         <v>1</v>
       </c>
       <c r="T12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -6305,11 +6290,8 @@
       <c r="F13" t="b">
         <v>1</v>
       </c>
-      <c r="H13" t="s">
-        <v>169</v>
-      </c>
       <c r="T13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -6335,10 +6317,10 @@
         <v>1</v>
       </c>
       <c r="T14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="U14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -6361,10 +6343,10 @@
         <v>42095</v>
       </c>
       <c r="T15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="U15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -6387,7 +6369,7 @@
         <v>6</v>
       </c>
       <c r="U16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -6413,10 +6395,10 @@
         <v>1</v>
       </c>
       <c r="T17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="U17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -6442,10 +6424,10 @@
         <v>1</v>
       </c>
       <c r="T18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="U18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -6468,10 +6450,10 @@
         <v>15.666</v>
       </c>
       <c r="T19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="U19" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -6491,16 +6473,16 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N20" t="b">
         <v>1</v>
       </c>
       <c r="T20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="U20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -6523,10 +6505,10 @@
         <v>7</v>
       </c>
       <c r="T21" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="U21" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -6555,7 +6537,7 @@
         <v>1</v>
       </c>
       <c r="T22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -6581,10 +6563,10 @@
         <v>10</v>
       </c>
       <c r="T23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="U23" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -6607,7 +6589,7 @@
         <v>11</v>
       </c>
       <c r="U24" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -6627,16 +6609,16 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="N25" t="b">
         <v>1</v>
       </c>
       <c r="T25" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="U25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -6656,16 +6638,16 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="N26" t="b">
         <v>1</v>
       </c>
       <c r="T26" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="U26" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="27" spans="1:21">
@@ -6685,13 +6667,13 @@
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="T27" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="U27" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -6717,10 +6699,10 @@
         <v>1</v>
       </c>
       <c r="T28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="U28" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:21">
@@ -6743,7 +6725,7 @@
         <v>1</v>
       </c>
       <c r="U29" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -6769,10 +6751,10 @@
         <v>10</v>
       </c>
       <c r="T30" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="U30" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -6798,10 +6780,10 @@
         <v>0</v>
       </c>
       <c r="T31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="U31" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:21">
@@ -6824,10 +6806,10 @@
         <v>12342151234</v>
       </c>
       <c r="T32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="U32" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:21">
@@ -6850,7 +6832,7 @@
         <v>12342151234</v>
       </c>
       <c r="U33" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:21">
@@ -6882,10 +6864,10 @@
         <v>1</v>
       </c>
       <c r="T34" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="U34" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:21">
@@ -6917,10 +6899,10 @@
         <v>1</v>
       </c>
       <c r="T35" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="U35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="36" spans="1:21">
@@ -6946,7 +6928,7 @@
         <v>1</v>
       </c>
       <c r="T36" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="37" spans="1:21">
@@ -6992,10 +6974,10 @@
         <v>1</v>
       </c>
       <c r="T38" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="U38" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" spans="1:21">
@@ -7018,10 +7000,10 @@
         <v>39</v>
       </c>
       <c r="T39" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="U39" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="40" spans="1:21">
@@ -7044,7 +7026,7 @@
         <v>40</v>
       </c>
       <c r="U40" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="41" spans="1:21">
@@ -7067,10 +7049,10 @@
         <v>41</v>
       </c>
       <c r="T41" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="U41" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:21">
@@ -7096,7 +7078,7 @@
         <v>1</v>
       </c>
       <c r="T42" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:21">
@@ -7119,7 +7101,7 @@
         <v>1</v>
       </c>
       <c r="T43" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:21">
@@ -7145,10 +7127,10 @@
         <v>0</v>
       </c>
       <c r="T44" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="U44" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:21">
@@ -7168,16 +7150,16 @@
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="O45" t="b">
         <v>0</v>
       </c>
       <c r="T45" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="U45" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:21">
@@ -7200,7 +7182,7 @@
         <v>1</v>
       </c>
       <c r="U46" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="47" spans="1:21">
@@ -7223,10 +7205,10 @@
         <v>1</v>
       </c>
       <c r="T47" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="U47" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="48" spans="1:21">
@@ -7252,18 +7234,18 @@
         <v>1</v>
       </c>
       <c r="T48" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="49" spans="1:21">
       <c r="A49" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B49" t="s">
         <v>166</v>
       </c>
       <c r="C49" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -7298,10 +7280,10 @@
         <v>145</v>
       </c>
       <c r="T50" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="U50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="51" spans="1:21">
@@ -7327,10 +7309,10 @@
         <v>29</v>
       </c>
       <c r="T51" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="U51" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="52" spans="1:21">
@@ -7362,7 +7344,7 @@
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
       <c r="U52" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="53" spans="1:21">
@@ -7397,10 +7379,10 @@
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
       <c r="T53" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="U53" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="54" spans="1:21">
@@ -7419,11 +7401,14 @@
       <c r="F54" t="b">
         <v>0</v>
       </c>
+      <c r="O54" t="b">
+        <v>1</v>
+      </c>
       <c r="T54" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="U54" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="55" spans="1:21">
@@ -7443,10 +7428,10 @@
         <v>1</v>
       </c>
       <c r="T55" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="U55" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="56" spans="1:21">
@@ -7472,10 +7457,10 @@
         <v>163</v>
       </c>
       <c r="T56" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="U56" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix validation of default ref entities
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/xls/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="14600" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18320" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="org_molgenis_test_TypeTest" sheetId="1" r:id="rId1"/>
@@ -5902,8 +5902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5914,8 +5914,9 @@
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8.5" customWidth="1"/>
     <col min="20" max="20" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -7246,7 +7247,7 @@
         <v>0</v>
       </c>
       <c r="F48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P48" t="b">
         <v>1</v>

</xml_diff>